<commit_message>
confirm seemingly successful implementation of master fnc and overwrite prism excel sheets
</commit_message>
<xml_diff>
--- a/data/230523-prism-dermis-output.xlsx
+++ b/data/230523-prism-dermis-output.xlsx
@@ -1068,6 +1068,156 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>23.54</v>
+      </c>
+      <c r="B2" t="n">
+        <v>37.18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>161.48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>34.32</v>
+      </c>
+      <c r="B3" t="n">
+        <v>25.52</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>27.94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>43.34</v>
+      </c>
+      <c r="C4" t="n">
+        <v>33.66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>26.18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>36.52</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35.86</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>16.06</v>
+      </c>
+      <c r="C6" t="n">
+        <v>106.48</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="n">
+        <v>57.97</v>
+      </c>
+      <c r="C7" t="n">
+        <v>29.48</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="n">
+        <v>32.56</v>
+      </c>
+      <c r="C8" t="n">
+        <v>97.24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" t="n">
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10" t="n">
+        <v>45.54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="n">
+        <v>21.34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" t="n">
+        <v>16.94</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="n">
+        <v>34.32</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" t="n">
+        <v>164.12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="n">
+        <v>23.32</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" t="n">
+        <v>78.76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" t="n">
+        <v>30.58</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="n">
+        <v>31.46</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" t="n">
+        <v>18.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>